<commit_message>
change excel exist path
</commit_message>
<xml_diff>
--- a/mypjt/date.xlsx
+++ b/mypjt/date.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ProgramsCode\GitHub\GraduationProject\ScrapyCode\GraduationProject\mypjt\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView activeTab="0" windowHeight="12645" windowWidth="22260" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="147">
   <si>
     <t>阿联酋迪拉姆</t>
   </si>
@@ -465,26 +460,27 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="等线"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="等线"/>
+      <charset val="134"/>
+      <family val="3"/>
       <sz val="9"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -500,24 +496,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="常规" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -783,25 +770,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:H55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="13.75" customWidth="1"/>
-    <col min="2" max="2" width="16.75" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="12.25" customWidth="1"/>
-    <col min="5" max="5" width="15.75" customWidth="1"/>
-    <col min="7" max="7" width="14.625" customWidth="1"/>
-    <col min="8" max="8" width="16.875" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" width="13.75"/>
+    <col customWidth="1" max="2" min="2" width="16.75"/>
+    <col customWidth="1" max="3" min="3" width="17"/>
+    <col customWidth="1" max="4" min="4" width="12.25"/>
+    <col customWidth="1" max="5" min="5" width="15.75"/>
+    <col customWidth="1" max="7" min="7" width="14.625"/>
+    <col customWidth="1" max="8" min="8" width="16.875"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -827,7 +818,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -853,7 +844,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -879,7 +870,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -905,7 +896,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -931,7 +922,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -957,7 +948,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -983,7 +974,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1009,7 +1000,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -1035,7 +1026,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -1061,7 +1052,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -1087,7 +1078,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -1113,7 +1104,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -1139,7 +1130,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>71</v>
       </c>
@@ -1165,7 +1156,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>77</v>
       </c>
@@ -1191,7 +1182,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>81</v>
       </c>
@@ -1217,7 +1208,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>86</v>
       </c>
@@ -1243,7 +1234,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>92</v>
       </c>
@@ -1269,7 +1260,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>98</v>
       </c>
@@ -1295,7 +1286,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>104</v>
       </c>
@@ -1321,7 +1312,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>108</v>
       </c>
@@ -1347,7 +1338,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>114</v>
       </c>
@@ -1373,7 +1364,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>120</v>
       </c>
@@ -1399,7 +1390,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>126</v>
       </c>
@@ -1425,7 +1416,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>132</v>
       </c>
@@ -1451,7 +1442,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>136</v>
       </c>
@@ -1477,7 +1468,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>141</v>
       </c>
@@ -1503,9 +1494,710 @@
         <v>6</v>
       </c>
     </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>3</v>
+      </c>
+      <c r="F29" t="s">
+        <v>4</v>
+      </c>
+      <c r="G29" t="s">
+        <v>5</v>
+      </c>
+      <c r="H29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" t="s">
+        <v>5</v>
+      </c>
+      <c r="H30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" t="s">
+        <v>5</v>
+      </c>
+      <c r="H31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" t="s">
+        <v>21</v>
+      </c>
+      <c r="F32" t="s">
+        <v>22</v>
+      </c>
+      <c r="G32" t="s">
+        <v>5</v>
+      </c>
+      <c r="H32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" t="s">
+        <v>27</v>
+      </c>
+      <c r="F33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G33" t="s">
+        <v>5</v>
+      </c>
+      <c r="H33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E34" t="s">
+        <v>33</v>
+      </c>
+      <c r="F34" t="s">
+        <v>34</v>
+      </c>
+      <c r="G34" t="s">
+        <v>5</v>
+      </c>
+      <c r="H34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" t="s">
+        <v>39</v>
+      </c>
+      <c r="F35" t="s">
+        <v>40</v>
+      </c>
+      <c r="G35" t="s">
+        <v>5</v>
+      </c>
+      <c r="H35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" t="s">
+        <v>44</v>
+      </c>
+      <c r="E36" t="s">
+        <v>45</v>
+      </c>
+      <c r="F36" t="s">
+        <v>46</v>
+      </c>
+      <c r="G36" t="s">
+        <v>5</v>
+      </c>
+      <c r="H36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37" t="s">
+        <v>50</v>
+      </c>
+      <c r="F37" t="s">
+        <v>51</v>
+      </c>
+      <c r="G37" t="s">
+        <v>5</v>
+      </c>
+      <c r="H37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>53</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
+        <v>54</v>
+      </c>
+      <c r="F38" t="s">
+        <v>55</v>
+      </c>
+      <c r="G38" t="s">
+        <v>5</v>
+      </c>
+      <c r="H38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>57</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1</v>
+      </c>
+      <c r="E39" t="s">
+        <v>58</v>
+      </c>
+      <c r="F39" t="s">
+        <v>59</v>
+      </c>
+      <c r="G39" t="s">
+        <v>5</v>
+      </c>
+      <c r="H39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" t="s">
+        <v>62</v>
+      </c>
+      <c r="D40" t="s">
+        <v>63</v>
+      </c>
+      <c r="E40" t="s">
+        <v>63</v>
+      </c>
+      <c r="F40" t="s">
+        <v>64</v>
+      </c>
+      <c r="G40" t="s">
+        <v>5</v>
+      </c>
+      <c r="H40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41" t="s">
+        <v>67</v>
+      </c>
+      <c r="D41" t="s">
+        <v>68</v>
+      </c>
+      <c r="E41" t="s">
+        <v>69</v>
+      </c>
+      <c r="F41" t="s">
+        <v>70</v>
+      </c>
+      <c r="G41" t="s">
+        <v>5</v>
+      </c>
+      <c r="H41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42" t="s">
+        <v>73</v>
+      </c>
+      <c r="D42" t="s">
+        <v>74</v>
+      </c>
+      <c r="E42" t="s">
+        <v>75</v>
+      </c>
+      <c r="F42" t="s">
+        <v>76</v>
+      </c>
+      <c r="G42" t="s">
+        <v>5</v>
+      </c>
+      <c r="H42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>79</v>
+      </c>
+      <c r="E43" t="s">
+        <v>1</v>
+      </c>
+      <c r="F43" t="s">
+        <v>80</v>
+      </c>
+      <c r="G43" t="s">
+        <v>5</v>
+      </c>
+      <c r="H43" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" t="s">
+        <v>81</v>
+      </c>
+      <c r="B44" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" t="s">
+        <v>83</v>
+      </c>
+      <c r="D44" t="s">
+        <v>84</v>
+      </c>
+      <c r="E44" t="s">
+        <v>85</v>
+      </c>
+      <c r="F44" t="s">
+        <v>51</v>
+      </c>
+      <c r="G44" t="s">
+        <v>5</v>
+      </c>
+      <c r="H44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" t="s">
+        <v>86</v>
+      </c>
+      <c r="B45" t="s">
+        <v>87</v>
+      </c>
+      <c r="C45" t="s">
+        <v>88</v>
+      </c>
+      <c r="D45" t="s">
+        <v>89</v>
+      </c>
+      <c r="E45" t="s">
+        <v>90</v>
+      </c>
+      <c r="F45" t="s">
+        <v>91</v>
+      </c>
+      <c r="G45" t="s">
+        <v>5</v>
+      </c>
+      <c r="H45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" t="s">
+        <v>92</v>
+      </c>
+      <c r="B46" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46" t="s">
+        <v>94</v>
+      </c>
+      <c r="D46" t="s">
+        <v>95</v>
+      </c>
+      <c r="E46" t="s">
+        <v>96</v>
+      </c>
+      <c r="F46" t="s">
+        <v>97</v>
+      </c>
+      <c r="G46" t="s">
+        <v>5</v>
+      </c>
+      <c r="H46" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47" t="s">
+        <v>100</v>
+      </c>
+      <c r="D47" t="s">
+        <v>101</v>
+      </c>
+      <c r="E47" t="s">
+        <v>102</v>
+      </c>
+      <c r="F47" t="s">
+        <v>103</v>
+      </c>
+      <c r="G47" t="s">
+        <v>5</v>
+      </c>
+      <c r="H47" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" t="s">
+        <v>104</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>105</v>
+      </c>
+      <c r="D48" t="s">
+        <v>1</v>
+      </c>
+      <c r="E48" t="s">
+        <v>106</v>
+      </c>
+      <c r="F48" t="s">
+        <v>107</v>
+      </c>
+      <c r="G48" t="s">
+        <v>5</v>
+      </c>
+      <c r="H48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" t="s">
+        <v>108</v>
+      </c>
+      <c r="B49" t="s">
+        <v>109</v>
+      </c>
+      <c r="C49" t="s">
+        <v>110</v>
+      </c>
+      <c r="D49" t="s">
+        <v>111</v>
+      </c>
+      <c r="E49" t="s">
+        <v>112</v>
+      </c>
+      <c r="F49" t="s">
+        <v>113</v>
+      </c>
+      <c r="G49" t="s">
+        <v>5</v>
+      </c>
+      <c r="H49" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" t="s">
+        <v>114</v>
+      </c>
+      <c r="B50" t="s">
+        <v>115</v>
+      </c>
+      <c r="C50" t="s">
+        <v>116</v>
+      </c>
+      <c r="D50" t="s">
+        <v>117</v>
+      </c>
+      <c r="E50" t="s">
+        <v>118</v>
+      </c>
+      <c r="F50" t="s">
+        <v>119</v>
+      </c>
+      <c r="G50" t="s">
+        <v>5</v>
+      </c>
+      <c r="H50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" t="s">
+        <v>120</v>
+      </c>
+      <c r="B51" t="s">
+        <v>121</v>
+      </c>
+      <c r="C51" t="s">
+        <v>122</v>
+      </c>
+      <c r="D51" t="s">
+        <v>123</v>
+      </c>
+      <c r="E51" t="s">
+        <v>124</v>
+      </c>
+      <c r="F51" t="s">
+        <v>125</v>
+      </c>
+      <c r="G51" t="s">
+        <v>5</v>
+      </c>
+      <c r="H51" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" t="s">
+        <v>126</v>
+      </c>
+      <c r="B52" t="s">
+        <v>127</v>
+      </c>
+      <c r="C52" t="s">
+        <v>128</v>
+      </c>
+      <c r="D52" t="s">
+        <v>129</v>
+      </c>
+      <c r="E52" t="s">
+        <v>130</v>
+      </c>
+      <c r="F52" t="s">
+        <v>131</v>
+      </c>
+      <c r="G52" t="s">
+        <v>5</v>
+      </c>
+      <c r="H52" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" t="s">
+        <v>132</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>133</v>
+      </c>
+      <c r="D53" t="s">
+        <v>1</v>
+      </c>
+      <c r="E53" t="s">
+        <v>134</v>
+      </c>
+      <c r="F53" t="s">
+        <v>135</v>
+      </c>
+      <c r="G53" t="s">
+        <v>5</v>
+      </c>
+      <c r="H53" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" t="s">
+        <v>136</v>
+      </c>
+      <c r="B54" t="s">
+        <v>137</v>
+      </c>
+      <c r="C54" t="s">
+        <v>138</v>
+      </c>
+      <c r="D54" t="s">
+        <v>139</v>
+      </c>
+      <c r="E54" t="s">
+        <v>139</v>
+      </c>
+      <c r="F54" t="s">
+        <v>140</v>
+      </c>
+      <c r="G54" t="s">
+        <v>5</v>
+      </c>
+      <c r="H54" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" t="s">
+        <v>141</v>
+      </c>
+      <c r="B55" t="s">
+        <v>142</v>
+      </c>
+      <c r="C55" t="s">
+        <v>143</v>
+      </c>
+      <c r="D55" t="s">
+        <v>144</v>
+      </c>
+      <c r="E55" t="s">
+        <v>145</v>
+      </c>
+      <c r="F55" t="s">
+        <v>146</v>
+      </c>
+      <c r="G55" t="s">
+        <v>5</v>
+      </c>
+      <c r="H55" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change excel save way
</commit_message>
<xml_diff>
--- a/mypjt/date.xlsx
+++ b/mypjt/date.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="212">
   <si>
     <t>阿联酋迪拉姆</t>
   </si>
@@ -455,6 +455,201 @@
   </si>
   <si>
     <t>53.29</t>
+  </si>
+  <si>
+    <t>166.4</t>
+  </si>
+  <si>
+    <t>178.48</t>
+  </si>
+  <si>
+    <t>2018-03-12</t>
+  </si>
+  <si>
+    <t>08:45:19</t>
+  </si>
+  <si>
+    <t>496.41</t>
+  </si>
+  <si>
+    <t>480.98</t>
+  </si>
+  <si>
+    <t>500.06</t>
+  </si>
+  <si>
+    <t>501.15</t>
+  </si>
+  <si>
+    <t>663.99</t>
+  </si>
+  <si>
+    <t>643.5</t>
+  </si>
+  <si>
+    <t>668.65</t>
+  </si>
+  <si>
+    <t>670.32</t>
+  </si>
+  <si>
+    <t>104.25</t>
+  </si>
+  <si>
+    <t>101.03</t>
+  </si>
+  <si>
+    <t>105.09</t>
+  </si>
+  <si>
+    <t>105.3</t>
+  </si>
+  <si>
+    <t>777.16</t>
+  </si>
+  <si>
+    <t>753.01</t>
+  </si>
+  <si>
+    <t>782.89</t>
+  </si>
+  <si>
+    <t>784.45</t>
+  </si>
+  <si>
+    <t>874.95</t>
+  </si>
+  <si>
+    <t>847.76</t>
+  </si>
+  <si>
+    <t>881.39</t>
+  </si>
+  <si>
+    <t>883.33</t>
+  </si>
+  <si>
+    <t>80.64</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>80.96</t>
+  </si>
+  <si>
+    <t>5.9058</t>
+  </si>
+  <si>
+    <t>5.7223</t>
+  </si>
+  <si>
+    <t>5.9492</t>
+  </si>
+  <si>
+    <t>0.5718</t>
+  </si>
+  <si>
+    <t>0.5974</t>
+  </si>
+  <si>
+    <t>0.6191</t>
+  </si>
+  <si>
+    <t>460.83</t>
+  </si>
+  <si>
+    <t>446.61</t>
+  </si>
+  <si>
+    <t>464.07</t>
+  </si>
+  <si>
+    <t>469.76</t>
+  </si>
+  <si>
+    <t>12.11</t>
+  </si>
+  <si>
+    <t>11.74</t>
+  </si>
+  <si>
+    <t>12.21</t>
+  </si>
+  <si>
+    <t>12.78</t>
+  </si>
+  <si>
+    <t>11.13</t>
+  </si>
+  <si>
+    <t>10.44</t>
+  </si>
+  <si>
+    <t>11.21</t>
+  </si>
+  <si>
+    <t>11.64</t>
+  </si>
+  <si>
+    <t>76.55</t>
+  </si>
+  <si>
+    <t>74.19</t>
+  </si>
+  <si>
+    <t>77.17</t>
+  </si>
+  <si>
+    <t>77.32</t>
+  </si>
+  <si>
+    <t>479.95</t>
+  </si>
+  <si>
+    <t>465.14</t>
+  </si>
+  <si>
+    <t>483.33</t>
+  </si>
+  <si>
+    <t>484.53</t>
+  </si>
+  <si>
+    <t>20.17</t>
+  </si>
+  <si>
+    <t>19.55</t>
+  </si>
+  <si>
+    <t>20.33</t>
+  </si>
+  <si>
+    <t>20.95</t>
+  </si>
+  <si>
+    <t>165.57</t>
+  </si>
+  <si>
+    <t>157.45</t>
+  </si>
+  <si>
+    <t>166.89</t>
+  </si>
+  <si>
+    <t>175.01</t>
+  </si>
+  <si>
+    <t>53.41</t>
+  </si>
+  <si>
+    <t>49.31</t>
+  </si>
+  <si>
+    <t>53.77</t>
+  </si>
+  <si>
+    <t>57.87</t>
   </si>
 </sst>
 </file>
@@ -775,7 +970,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:H55"/>
+  <dimension ref="A2:H163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
@@ -2196,6 +2391,2814 @@
         <v>6</v>
       </c>
     </row>
+    <row r="56" spans="1:8">
+      <c r="A56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>147</v>
+      </c>
+      <c r="D56" t="s">
+        <v>1</v>
+      </c>
+      <c r="E56" t="s">
+        <v>148</v>
+      </c>
+      <c r="F56" t="s">
+        <v>4</v>
+      </c>
+      <c r="G56" t="s">
+        <v>149</v>
+      </c>
+      <c r="H56" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" t="s">
+        <v>151</v>
+      </c>
+      <c r="C57" t="s">
+        <v>152</v>
+      </c>
+      <c r="D57" t="s">
+        <v>153</v>
+      </c>
+      <c r="E57" t="s">
+        <v>154</v>
+      </c>
+      <c r="F57" t="s">
+        <v>12</v>
+      </c>
+      <c r="G57" t="s">
+        <v>149</v>
+      </c>
+      <c r="H57" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" t="s">
+        <v>13</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" t="s">
+        <v>1</v>
+      </c>
+      <c r="E58" t="s">
+        <v>15</v>
+      </c>
+      <c r="F58" t="s">
+        <v>16</v>
+      </c>
+      <c r="G58" t="s">
+        <v>149</v>
+      </c>
+      <c r="H58" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" t="s">
+        <v>17</v>
+      </c>
+      <c r="B59" t="s">
+        <v>18</v>
+      </c>
+      <c r="C59" t="s">
+        <v>19</v>
+      </c>
+      <c r="D59" t="s">
+        <v>20</v>
+      </c>
+      <c r="E59" t="s">
+        <v>21</v>
+      </c>
+      <c r="F59" t="s">
+        <v>22</v>
+      </c>
+      <c r="G59" t="s">
+        <v>149</v>
+      </c>
+      <c r="H59" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" t="s">
+        <v>23</v>
+      </c>
+      <c r="B60" t="s">
+        <v>155</v>
+      </c>
+      <c r="C60" t="s">
+        <v>156</v>
+      </c>
+      <c r="D60" t="s">
+        <v>157</v>
+      </c>
+      <c r="E60" t="s">
+        <v>158</v>
+      </c>
+      <c r="F60" t="s">
+        <v>28</v>
+      </c>
+      <c r="G60" t="s">
+        <v>149</v>
+      </c>
+      <c r="H60" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" t="s">
+        <v>29</v>
+      </c>
+      <c r="B61" t="s">
+        <v>159</v>
+      </c>
+      <c r="C61" t="s">
+        <v>160</v>
+      </c>
+      <c r="D61" t="s">
+        <v>161</v>
+      </c>
+      <c r="E61" t="s">
+        <v>162</v>
+      </c>
+      <c r="F61" t="s">
+        <v>34</v>
+      </c>
+      <c r="G61" t="s">
+        <v>149</v>
+      </c>
+      <c r="H61" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" t="s">
+        <v>35</v>
+      </c>
+      <c r="B62" t="s">
+        <v>163</v>
+      </c>
+      <c r="C62" t="s">
+        <v>164</v>
+      </c>
+      <c r="D62" t="s">
+        <v>165</v>
+      </c>
+      <c r="E62" t="s">
+        <v>166</v>
+      </c>
+      <c r="F62" t="s">
+        <v>40</v>
+      </c>
+      <c r="G62" t="s">
+        <v>149</v>
+      </c>
+      <c r="H62" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" t="s">
+        <v>41</v>
+      </c>
+      <c r="B63" t="s">
+        <v>167</v>
+      </c>
+      <c r="C63" t="s">
+        <v>168</v>
+      </c>
+      <c r="D63" t="s">
+        <v>169</v>
+      </c>
+      <c r="E63" t="s">
+        <v>170</v>
+      </c>
+      <c r="F63" t="s">
+        <v>46</v>
+      </c>
+      <c r="G63" t="s">
+        <v>149</v>
+      </c>
+      <c r="H63" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" t="s">
+        <v>47</v>
+      </c>
+      <c r="B64" t="s">
+        <v>171</v>
+      </c>
+      <c r="C64" t="s">
+        <v>172</v>
+      </c>
+      <c r="D64" t="s">
+        <v>173</v>
+      </c>
+      <c r="E64" t="s">
+        <v>173</v>
+      </c>
+      <c r="F64" t="s">
+        <v>51</v>
+      </c>
+      <c r="G64" t="s">
+        <v>149</v>
+      </c>
+      <c r="H64" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" t="s">
+        <v>52</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" t="s">
+        <v>53</v>
+      </c>
+      <c r="D65" t="s">
+        <v>1</v>
+      </c>
+      <c r="E65" t="s">
+        <v>54</v>
+      </c>
+      <c r="F65" t="s">
+        <v>55</v>
+      </c>
+      <c r="G65" t="s">
+        <v>149</v>
+      </c>
+      <c r="H65" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" t="s">
+        <v>56</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D66" t="s">
+        <v>1</v>
+      </c>
+      <c r="E66" t="s">
+        <v>58</v>
+      </c>
+      <c r="F66" t="s">
+        <v>59</v>
+      </c>
+      <c r="G66" t="s">
+        <v>149</v>
+      </c>
+      <c r="H66" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" t="s">
+        <v>60</v>
+      </c>
+      <c r="B67" t="s">
+        <v>174</v>
+      </c>
+      <c r="C67" t="s">
+        <v>175</v>
+      </c>
+      <c r="D67" t="s">
+        <v>176</v>
+      </c>
+      <c r="E67" t="s">
+        <v>176</v>
+      </c>
+      <c r="F67" t="s">
+        <v>64</v>
+      </c>
+      <c r="G67" t="s">
+        <v>149</v>
+      </c>
+      <c r="H67" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" t="s">
+        <v>65</v>
+      </c>
+      <c r="B68" t="s">
+        <v>70</v>
+      </c>
+      <c r="C68" t="s">
+        <v>177</v>
+      </c>
+      <c r="D68" t="s">
+        <v>178</v>
+      </c>
+      <c r="E68" t="s">
+        <v>179</v>
+      </c>
+      <c r="F68" t="s">
+        <v>70</v>
+      </c>
+      <c r="G68" t="s">
+        <v>149</v>
+      </c>
+      <c r="H68" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" t="s">
+        <v>71</v>
+      </c>
+      <c r="B69" t="s">
+        <v>72</v>
+      </c>
+      <c r="C69" t="s">
+        <v>73</v>
+      </c>
+      <c r="D69" t="s">
+        <v>74</v>
+      </c>
+      <c r="E69" t="s">
+        <v>75</v>
+      </c>
+      <c r="F69" t="s">
+        <v>76</v>
+      </c>
+      <c r="G69" t="s">
+        <v>149</v>
+      </c>
+      <c r="H69" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" t="s">
+        <v>77</v>
+      </c>
+      <c r="B70" t="s">
+        <v>78</v>
+      </c>
+      <c r="C70" t="s">
+        <v>1</v>
+      </c>
+      <c r="D70" t="s">
+        <v>79</v>
+      </c>
+      <c r="E70" t="s">
+        <v>1</v>
+      </c>
+      <c r="F70" t="s">
+        <v>80</v>
+      </c>
+      <c r="G70" t="s">
+        <v>149</v>
+      </c>
+      <c r="H70" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" t="s">
+        <v>81</v>
+      </c>
+      <c r="B71" t="s">
+        <v>82</v>
+      </c>
+      <c r="C71" t="s">
+        <v>83</v>
+      </c>
+      <c r="D71" t="s">
+        <v>84</v>
+      </c>
+      <c r="E71" t="s">
+        <v>85</v>
+      </c>
+      <c r="F71" t="s">
+        <v>51</v>
+      </c>
+      <c r="G71" t="s">
+        <v>149</v>
+      </c>
+      <c r="H71" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" t="s">
+        <v>86</v>
+      </c>
+      <c r="B72" t="s">
+        <v>180</v>
+      </c>
+      <c r="C72" t="s">
+        <v>181</v>
+      </c>
+      <c r="D72" t="s">
+        <v>182</v>
+      </c>
+      <c r="E72" t="s">
+        <v>183</v>
+      </c>
+      <c r="F72" t="s">
+        <v>91</v>
+      </c>
+      <c r="G72" t="s">
+        <v>149</v>
+      </c>
+      <c r="H72" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" t="s">
+        <v>92</v>
+      </c>
+      <c r="B73" t="s">
+        <v>184</v>
+      </c>
+      <c r="C73" t="s">
+        <v>185</v>
+      </c>
+      <c r="D73" t="s">
+        <v>186</v>
+      </c>
+      <c r="E73" t="s">
+        <v>187</v>
+      </c>
+      <c r="F73" t="s">
+        <v>97</v>
+      </c>
+      <c r="G73" t="s">
+        <v>149</v>
+      </c>
+      <c r="H73" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" t="s">
+        <v>98</v>
+      </c>
+      <c r="B74" t="s">
+        <v>188</v>
+      </c>
+      <c r="C74" t="s">
+        <v>189</v>
+      </c>
+      <c r="D74" t="s">
+        <v>190</v>
+      </c>
+      <c r="E74" t="s">
+        <v>191</v>
+      </c>
+      <c r="F74" t="s">
+        <v>103</v>
+      </c>
+      <c r="G74" t="s">
+        <v>149</v>
+      </c>
+      <c r="H74" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" t="s">
+        <v>104</v>
+      </c>
+      <c r="B75" t="s">
+        <v>1</v>
+      </c>
+      <c r="C75" t="s">
+        <v>105</v>
+      </c>
+      <c r="D75" t="s">
+        <v>1</v>
+      </c>
+      <c r="E75" t="s">
+        <v>106</v>
+      </c>
+      <c r="F75" t="s">
+        <v>107</v>
+      </c>
+      <c r="G75" t="s">
+        <v>149</v>
+      </c>
+      <c r="H75" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" t="s">
+        <v>108</v>
+      </c>
+      <c r="B76" t="s">
+        <v>192</v>
+      </c>
+      <c r="C76" t="s">
+        <v>193</v>
+      </c>
+      <c r="D76" t="s">
+        <v>194</v>
+      </c>
+      <c r="E76" t="s">
+        <v>195</v>
+      </c>
+      <c r="F76" t="s">
+        <v>113</v>
+      </c>
+      <c r="G76" t="s">
+        <v>149</v>
+      </c>
+      <c r="H76" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" t="s">
+        <v>114</v>
+      </c>
+      <c r="B77" t="s">
+        <v>196</v>
+      </c>
+      <c r="C77" t="s">
+        <v>197</v>
+      </c>
+      <c r="D77" t="s">
+        <v>198</v>
+      </c>
+      <c r="E77" t="s">
+        <v>199</v>
+      </c>
+      <c r="F77" t="s">
+        <v>119</v>
+      </c>
+      <c r="G77" t="s">
+        <v>149</v>
+      </c>
+      <c r="H77" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" t="s">
+        <v>120</v>
+      </c>
+      <c r="B78" t="s">
+        <v>200</v>
+      </c>
+      <c r="C78" t="s">
+        <v>201</v>
+      </c>
+      <c r="D78" t="s">
+        <v>202</v>
+      </c>
+      <c r="E78" t="s">
+        <v>203</v>
+      </c>
+      <c r="F78" t="s">
+        <v>125</v>
+      </c>
+      <c r="G78" t="s">
+        <v>149</v>
+      </c>
+      <c r="H78" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79" t="s">
+        <v>126</v>
+      </c>
+      <c r="B79" t="s">
+        <v>204</v>
+      </c>
+      <c r="C79" t="s">
+        <v>205</v>
+      </c>
+      <c r="D79" t="s">
+        <v>206</v>
+      </c>
+      <c r="E79" t="s">
+        <v>207</v>
+      </c>
+      <c r="F79" t="s">
+        <v>131</v>
+      </c>
+      <c r="G79" t="s">
+        <v>149</v>
+      </c>
+      <c r="H79" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" t="s">
+        <v>132</v>
+      </c>
+      <c r="B80" t="s">
+        <v>1</v>
+      </c>
+      <c r="C80" t="s">
+        <v>133</v>
+      </c>
+      <c r="D80" t="s">
+        <v>1</v>
+      </c>
+      <c r="E80" t="s">
+        <v>134</v>
+      </c>
+      <c r="F80" t="s">
+        <v>135</v>
+      </c>
+      <c r="G80" t="s">
+        <v>149</v>
+      </c>
+      <c r="H80" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" t="s">
+        <v>136</v>
+      </c>
+      <c r="B81" t="s">
+        <v>137</v>
+      </c>
+      <c r="C81" t="s">
+        <v>138</v>
+      </c>
+      <c r="D81" t="s">
+        <v>139</v>
+      </c>
+      <c r="E81" t="s">
+        <v>139</v>
+      </c>
+      <c r="F81" t="s">
+        <v>140</v>
+      </c>
+      <c r="G81" t="s">
+        <v>149</v>
+      </c>
+      <c r="H81" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82" t="s">
+        <v>141</v>
+      </c>
+      <c r="B82" t="s">
+        <v>208</v>
+      </c>
+      <c r="C82" t="s">
+        <v>209</v>
+      </c>
+      <c r="D82" t="s">
+        <v>210</v>
+      </c>
+      <c r="E82" t="s">
+        <v>211</v>
+      </c>
+      <c r="F82" t="s">
+        <v>146</v>
+      </c>
+      <c r="G82" t="s">
+        <v>149</v>
+      </c>
+      <c r="H82" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83" t="s">
+        <v>0</v>
+      </c>
+      <c r="B83" t="s">
+        <v>1</v>
+      </c>
+      <c r="C83" t="s">
+        <v>147</v>
+      </c>
+      <c r="D83" t="s">
+        <v>1</v>
+      </c>
+      <c r="E83" t="s">
+        <v>148</v>
+      </c>
+      <c r="F83" t="s">
+        <v>4</v>
+      </c>
+      <c r="G83" t="s">
+        <v>149</v>
+      </c>
+      <c r="H83" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8">
+      <c r="A84" t="s">
+        <v>7</v>
+      </c>
+      <c r="B84" t="s">
+        <v>151</v>
+      </c>
+      <c r="C84" t="s">
+        <v>152</v>
+      </c>
+      <c r="D84" t="s">
+        <v>153</v>
+      </c>
+      <c r="E84" t="s">
+        <v>154</v>
+      </c>
+      <c r="F84" t="s">
+        <v>12</v>
+      </c>
+      <c r="G84" t="s">
+        <v>149</v>
+      </c>
+      <c r="H84" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8">
+      <c r="A85" t="s">
+        <v>13</v>
+      </c>
+      <c r="B85" t="s">
+        <v>1</v>
+      </c>
+      <c r="C85" t="s">
+        <v>14</v>
+      </c>
+      <c r="D85" t="s">
+        <v>1</v>
+      </c>
+      <c r="E85" t="s">
+        <v>15</v>
+      </c>
+      <c r="F85" t="s">
+        <v>16</v>
+      </c>
+      <c r="G85" t="s">
+        <v>149</v>
+      </c>
+      <c r="H85" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="A86" t="s">
+        <v>17</v>
+      </c>
+      <c r="B86" t="s">
+        <v>18</v>
+      </c>
+      <c r="C86" t="s">
+        <v>19</v>
+      </c>
+      <c r="D86" t="s">
+        <v>20</v>
+      </c>
+      <c r="E86" t="s">
+        <v>21</v>
+      </c>
+      <c r="F86" t="s">
+        <v>22</v>
+      </c>
+      <c r="G86" t="s">
+        <v>149</v>
+      </c>
+      <c r="H86" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="A87" t="s">
+        <v>23</v>
+      </c>
+      <c r="B87" t="s">
+        <v>155</v>
+      </c>
+      <c r="C87" t="s">
+        <v>156</v>
+      </c>
+      <c r="D87" t="s">
+        <v>157</v>
+      </c>
+      <c r="E87" t="s">
+        <v>158</v>
+      </c>
+      <c r="F87" t="s">
+        <v>28</v>
+      </c>
+      <c r="G87" t="s">
+        <v>149</v>
+      </c>
+      <c r="H87" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8">
+      <c r="A88" t="s">
+        <v>29</v>
+      </c>
+      <c r="B88" t="s">
+        <v>159</v>
+      </c>
+      <c r="C88" t="s">
+        <v>160</v>
+      </c>
+      <c r="D88" t="s">
+        <v>161</v>
+      </c>
+      <c r="E88" t="s">
+        <v>162</v>
+      </c>
+      <c r="F88" t="s">
+        <v>34</v>
+      </c>
+      <c r="G88" t="s">
+        <v>149</v>
+      </c>
+      <c r="H88" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8">
+      <c r="A89" t="s">
+        <v>35</v>
+      </c>
+      <c r="B89" t="s">
+        <v>163</v>
+      </c>
+      <c r="C89" t="s">
+        <v>164</v>
+      </c>
+      <c r="D89" t="s">
+        <v>165</v>
+      </c>
+      <c r="E89" t="s">
+        <v>166</v>
+      </c>
+      <c r="F89" t="s">
+        <v>40</v>
+      </c>
+      <c r="G89" t="s">
+        <v>149</v>
+      </c>
+      <c r="H89" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="A90" t="s">
+        <v>41</v>
+      </c>
+      <c r="B90" t="s">
+        <v>167</v>
+      </c>
+      <c r="C90" t="s">
+        <v>168</v>
+      </c>
+      <c r="D90" t="s">
+        <v>169</v>
+      </c>
+      <c r="E90" t="s">
+        <v>170</v>
+      </c>
+      <c r="F90" t="s">
+        <v>46</v>
+      </c>
+      <c r="G90" t="s">
+        <v>149</v>
+      </c>
+      <c r="H90" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8">
+      <c r="A91" t="s">
+        <v>47</v>
+      </c>
+      <c r="B91" t="s">
+        <v>171</v>
+      </c>
+      <c r="C91" t="s">
+        <v>172</v>
+      </c>
+      <c r="D91" t="s">
+        <v>173</v>
+      </c>
+      <c r="E91" t="s">
+        <v>173</v>
+      </c>
+      <c r="F91" t="s">
+        <v>51</v>
+      </c>
+      <c r="G91" t="s">
+        <v>149</v>
+      </c>
+      <c r="H91" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8">
+      <c r="A92" t="s">
+        <v>52</v>
+      </c>
+      <c r="B92" t="s">
+        <v>1</v>
+      </c>
+      <c r="C92" t="s">
+        <v>53</v>
+      </c>
+      <c r="D92" t="s">
+        <v>1</v>
+      </c>
+      <c r="E92" t="s">
+        <v>54</v>
+      </c>
+      <c r="F92" t="s">
+        <v>55</v>
+      </c>
+      <c r="G92" t="s">
+        <v>149</v>
+      </c>
+      <c r="H92" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8">
+      <c r="A93" t="s">
+        <v>56</v>
+      </c>
+      <c r="B93" t="s">
+        <v>1</v>
+      </c>
+      <c r="C93" t="s">
+        <v>57</v>
+      </c>
+      <c r="D93" t="s">
+        <v>1</v>
+      </c>
+      <c r="E93" t="s">
+        <v>58</v>
+      </c>
+      <c r="F93" t="s">
+        <v>59</v>
+      </c>
+      <c r="G93" t="s">
+        <v>149</v>
+      </c>
+      <c r="H93" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8">
+      <c r="A94" t="s">
+        <v>60</v>
+      </c>
+      <c r="B94" t="s">
+        <v>174</v>
+      </c>
+      <c r="C94" t="s">
+        <v>175</v>
+      </c>
+      <c r="D94" t="s">
+        <v>176</v>
+      </c>
+      <c r="E94" t="s">
+        <v>176</v>
+      </c>
+      <c r="F94" t="s">
+        <v>64</v>
+      </c>
+      <c r="G94" t="s">
+        <v>149</v>
+      </c>
+      <c r="H94" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8">
+      <c r="A95" t="s">
+        <v>65</v>
+      </c>
+      <c r="B95" t="s">
+        <v>70</v>
+      </c>
+      <c r="C95" t="s">
+        <v>177</v>
+      </c>
+      <c r="D95" t="s">
+        <v>178</v>
+      </c>
+      <c r="E95" t="s">
+        <v>179</v>
+      </c>
+      <c r="F95" t="s">
+        <v>70</v>
+      </c>
+      <c r="G95" t="s">
+        <v>149</v>
+      </c>
+      <c r="H95" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8">
+      <c r="A96" t="s">
+        <v>71</v>
+      </c>
+      <c r="B96" t="s">
+        <v>72</v>
+      </c>
+      <c r="C96" t="s">
+        <v>73</v>
+      </c>
+      <c r="D96" t="s">
+        <v>74</v>
+      </c>
+      <c r="E96" t="s">
+        <v>75</v>
+      </c>
+      <c r="F96" t="s">
+        <v>76</v>
+      </c>
+      <c r="G96" t="s">
+        <v>149</v>
+      </c>
+      <c r="H96" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8">
+      <c r="A97" t="s">
+        <v>77</v>
+      </c>
+      <c r="B97" t="s">
+        <v>78</v>
+      </c>
+      <c r="C97" t="s">
+        <v>1</v>
+      </c>
+      <c r="D97" t="s">
+        <v>79</v>
+      </c>
+      <c r="E97" t="s">
+        <v>1</v>
+      </c>
+      <c r="F97" t="s">
+        <v>80</v>
+      </c>
+      <c r="G97" t="s">
+        <v>149</v>
+      </c>
+      <c r="H97" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8">
+      <c r="A98" t="s">
+        <v>81</v>
+      </c>
+      <c r="B98" t="s">
+        <v>82</v>
+      </c>
+      <c r="C98" t="s">
+        <v>83</v>
+      </c>
+      <c r="D98" t="s">
+        <v>84</v>
+      </c>
+      <c r="E98" t="s">
+        <v>85</v>
+      </c>
+      <c r="F98" t="s">
+        <v>51</v>
+      </c>
+      <c r="G98" t="s">
+        <v>149</v>
+      </c>
+      <c r="H98" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8">
+      <c r="A99" t="s">
+        <v>86</v>
+      </c>
+      <c r="B99" t="s">
+        <v>180</v>
+      </c>
+      <c r="C99" t="s">
+        <v>181</v>
+      </c>
+      <c r="D99" t="s">
+        <v>182</v>
+      </c>
+      <c r="E99" t="s">
+        <v>183</v>
+      </c>
+      <c r="F99" t="s">
+        <v>91</v>
+      </c>
+      <c r="G99" t="s">
+        <v>149</v>
+      </c>
+      <c r="H99" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8">
+      <c r="A100" t="s">
+        <v>92</v>
+      </c>
+      <c r="B100" t="s">
+        <v>184</v>
+      </c>
+      <c r="C100" t="s">
+        <v>185</v>
+      </c>
+      <c r="D100" t="s">
+        <v>186</v>
+      </c>
+      <c r="E100" t="s">
+        <v>187</v>
+      </c>
+      <c r="F100" t="s">
+        <v>97</v>
+      </c>
+      <c r="G100" t="s">
+        <v>149</v>
+      </c>
+      <c r="H100" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8">
+      <c r="A101" t="s">
+        <v>98</v>
+      </c>
+      <c r="B101" t="s">
+        <v>188</v>
+      </c>
+      <c r="C101" t="s">
+        <v>189</v>
+      </c>
+      <c r="D101" t="s">
+        <v>190</v>
+      </c>
+      <c r="E101" t="s">
+        <v>191</v>
+      </c>
+      <c r="F101" t="s">
+        <v>103</v>
+      </c>
+      <c r="G101" t="s">
+        <v>149</v>
+      </c>
+      <c r="H101" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8">
+      <c r="A102" t="s">
+        <v>104</v>
+      </c>
+      <c r="B102" t="s">
+        <v>1</v>
+      </c>
+      <c r="C102" t="s">
+        <v>105</v>
+      </c>
+      <c r="D102" t="s">
+        <v>1</v>
+      </c>
+      <c r="E102" t="s">
+        <v>106</v>
+      </c>
+      <c r="F102" t="s">
+        <v>107</v>
+      </c>
+      <c r="G102" t="s">
+        <v>149</v>
+      </c>
+      <c r="H102" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8">
+      <c r="A103" t="s">
+        <v>108</v>
+      </c>
+      <c r="B103" t="s">
+        <v>192</v>
+      </c>
+      <c r="C103" t="s">
+        <v>193</v>
+      </c>
+      <c r="D103" t="s">
+        <v>194</v>
+      </c>
+      <c r="E103" t="s">
+        <v>195</v>
+      </c>
+      <c r="F103" t="s">
+        <v>113</v>
+      </c>
+      <c r="G103" t="s">
+        <v>149</v>
+      </c>
+      <c r="H103" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8">
+      <c r="A104" t="s">
+        <v>114</v>
+      </c>
+      <c r="B104" t="s">
+        <v>196</v>
+      </c>
+      <c r="C104" t="s">
+        <v>197</v>
+      </c>
+      <c r="D104" t="s">
+        <v>198</v>
+      </c>
+      <c r="E104" t="s">
+        <v>199</v>
+      </c>
+      <c r="F104" t="s">
+        <v>119</v>
+      </c>
+      <c r="G104" t="s">
+        <v>149</v>
+      </c>
+      <c r="H104" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8">
+      <c r="A105" t="s">
+        <v>120</v>
+      </c>
+      <c r="B105" t="s">
+        <v>200</v>
+      </c>
+      <c r="C105" t="s">
+        <v>201</v>
+      </c>
+      <c r="D105" t="s">
+        <v>202</v>
+      </c>
+      <c r="E105" t="s">
+        <v>203</v>
+      </c>
+      <c r="F105" t="s">
+        <v>125</v>
+      </c>
+      <c r="G105" t="s">
+        <v>149</v>
+      </c>
+      <c r="H105" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8">
+      <c r="A106" t="s">
+        <v>126</v>
+      </c>
+      <c r="B106" t="s">
+        <v>204</v>
+      </c>
+      <c r="C106" t="s">
+        <v>205</v>
+      </c>
+      <c r="D106" t="s">
+        <v>206</v>
+      </c>
+      <c r="E106" t="s">
+        <v>207</v>
+      </c>
+      <c r="F106" t="s">
+        <v>131</v>
+      </c>
+      <c r="G106" t="s">
+        <v>149</v>
+      </c>
+      <c r="H106" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8">
+      <c r="A107" t="s">
+        <v>132</v>
+      </c>
+      <c r="B107" t="s">
+        <v>1</v>
+      </c>
+      <c r="C107" t="s">
+        <v>133</v>
+      </c>
+      <c r="D107" t="s">
+        <v>1</v>
+      </c>
+      <c r="E107" t="s">
+        <v>134</v>
+      </c>
+      <c r="F107" t="s">
+        <v>135</v>
+      </c>
+      <c r="G107" t="s">
+        <v>149</v>
+      </c>
+      <c r="H107" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8">
+      <c r="A108" t="s">
+        <v>136</v>
+      </c>
+      <c r="B108" t="s">
+        <v>137</v>
+      </c>
+      <c r="C108" t="s">
+        <v>138</v>
+      </c>
+      <c r="D108" t="s">
+        <v>139</v>
+      </c>
+      <c r="E108" t="s">
+        <v>139</v>
+      </c>
+      <c r="F108" t="s">
+        <v>140</v>
+      </c>
+      <c r="G108" t="s">
+        <v>149</v>
+      </c>
+      <c r="H108" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8">
+      <c r="A109" t="s">
+        <v>141</v>
+      </c>
+      <c r="B109" t="s">
+        <v>208</v>
+      </c>
+      <c r="C109" t="s">
+        <v>209</v>
+      </c>
+      <c r="D109" t="s">
+        <v>210</v>
+      </c>
+      <c r="E109" t="s">
+        <v>211</v>
+      </c>
+      <c r="F109" t="s">
+        <v>146</v>
+      </c>
+      <c r="G109" t="s">
+        <v>149</v>
+      </c>
+      <c r="H109" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8">
+      <c r="A110" t="s">
+        <v>0</v>
+      </c>
+      <c r="B110" t="s">
+        <v>1</v>
+      </c>
+      <c r="C110" t="s">
+        <v>147</v>
+      </c>
+      <c r="D110" t="s">
+        <v>1</v>
+      </c>
+      <c r="E110" t="s">
+        <v>148</v>
+      </c>
+      <c r="F110" t="s">
+        <v>4</v>
+      </c>
+      <c r="G110" t="s">
+        <v>149</v>
+      </c>
+      <c r="H110" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8">
+      <c r="A111" t="s">
+        <v>7</v>
+      </c>
+      <c r="B111" t="s">
+        <v>151</v>
+      </c>
+      <c r="C111" t="s">
+        <v>152</v>
+      </c>
+      <c r="D111" t="s">
+        <v>153</v>
+      </c>
+      <c r="E111" t="s">
+        <v>154</v>
+      </c>
+      <c r="F111" t="s">
+        <v>12</v>
+      </c>
+      <c r="G111" t="s">
+        <v>149</v>
+      </c>
+      <c r="H111" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8">
+      <c r="A112" t="s">
+        <v>13</v>
+      </c>
+      <c r="B112" t="s">
+        <v>1</v>
+      </c>
+      <c r="C112" t="s">
+        <v>14</v>
+      </c>
+      <c r="D112" t="s">
+        <v>1</v>
+      </c>
+      <c r="E112" t="s">
+        <v>15</v>
+      </c>
+      <c r="F112" t="s">
+        <v>16</v>
+      </c>
+      <c r="G112" t="s">
+        <v>149</v>
+      </c>
+      <c r="H112" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8">
+      <c r="A113" t="s">
+        <v>17</v>
+      </c>
+      <c r="B113" t="s">
+        <v>18</v>
+      </c>
+      <c r="C113" t="s">
+        <v>19</v>
+      </c>
+      <c r="D113" t="s">
+        <v>20</v>
+      </c>
+      <c r="E113" t="s">
+        <v>21</v>
+      </c>
+      <c r="F113" t="s">
+        <v>22</v>
+      </c>
+      <c r="G113" t="s">
+        <v>149</v>
+      </c>
+      <c r="H113" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8">
+      <c r="A114" t="s">
+        <v>23</v>
+      </c>
+      <c r="B114" t="s">
+        <v>155</v>
+      </c>
+      <c r="C114" t="s">
+        <v>156</v>
+      </c>
+      <c r="D114" t="s">
+        <v>157</v>
+      </c>
+      <c r="E114" t="s">
+        <v>158</v>
+      </c>
+      <c r="F114" t="s">
+        <v>28</v>
+      </c>
+      <c r="G114" t="s">
+        <v>149</v>
+      </c>
+      <c r="H114" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8">
+      <c r="A115" t="s">
+        <v>29</v>
+      </c>
+      <c r="B115" t="s">
+        <v>159</v>
+      </c>
+      <c r="C115" t="s">
+        <v>160</v>
+      </c>
+      <c r="D115" t="s">
+        <v>161</v>
+      </c>
+      <c r="E115" t="s">
+        <v>162</v>
+      </c>
+      <c r="F115" t="s">
+        <v>34</v>
+      </c>
+      <c r="G115" t="s">
+        <v>149</v>
+      </c>
+      <c r="H115" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8">
+      <c r="A116" t="s">
+        <v>35</v>
+      </c>
+      <c r="B116" t="s">
+        <v>163</v>
+      </c>
+      <c r="C116" t="s">
+        <v>164</v>
+      </c>
+      <c r="D116" t="s">
+        <v>165</v>
+      </c>
+      <c r="E116" t="s">
+        <v>166</v>
+      </c>
+      <c r="F116" t="s">
+        <v>40</v>
+      </c>
+      <c r="G116" t="s">
+        <v>149</v>
+      </c>
+      <c r="H116" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8">
+      <c r="A117" t="s">
+        <v>41</v>
+      </c>
+      <c r="B117" t="s">
+        <v>167</v>
+      </c>
+      <c r="C117" t="s">
+        <v>168</v>
+      </c>
+      <c r="D117" t="s">
+        <v>169</v>
+      </c>
+      <c r="E117" t="s">
+        <v>170</v>
+      </c>
+      <c r="F117" t="s">
+        <v>46</v>
+      </c>
+      <c r="G117" t="s">
+        <v>149</v>
+      </c>
+      <c r="H117" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8">
+      <c r="A118" t="s">
+        <v>47</v>
+      </c>
+      <c r="B118" t="s">
+        <v>171</v>
+      </c>
+      <c r="C118" t="s">
+        <v>172</v>
+      </c>
+      <c r="D118" t="s">
+        <v>173</v>
+      </c>
+      <c r="E118" t="s">
+        <v>173</v>
+      </c>
+      <c r="F118" t="s">
+        <v>51</v>
+      </c>
+      <c r="G118" t="s">
+        <v>149</v>
+      </c>
+      <c r="H118" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8">
+      <c r="A119" t="s">
+        <v>52</v>
+      </c>
+      <c r="B119" t="s">
+        <v>1</v>
+      </c>
+      <c r="C119" t="s">
+        <v>53</v>
+      </c>
+      <c r="D119" t="s">
+        <v>1</v>
+      </c>
+      <c r="E119" t="s">
+        <v>54</v>
+      </c>
+      <c r="F119" t="s">
+        <v>55</v>
+      </c>
+      <c r="G119" t="s">
+        <v>149</v>
+      </c>
+      <c r="H119" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8">
+      <c r="A120" t="s">
+        <v>56</v>
+      </c>
+      <c r="B120" t="s">
+        <v>1</v>
+      </c>
+      <c r="C120" t="s">
+        <v>57</v>
+      </c>
+      <c r="D120" t="s">
+        <v>1</v>
+      </c>
+      <c r="E120" t="s">
+        <v>58</v>
+      </c>
+      <c r="F120" t="s">
+        <v>59</v>
+      </c>
+      <c r="G120" t="s">
+        <v>149</v>
+      </c>
+      <c r="H120" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8">
+      <c r="A121" t="s">
+        <v>60</v>
+      </c>
+      <c r="B121" t="s">
+        <v>174</v>
+      </c>
+      <c r="C121" t="s">
+        <v>175</v>
+      </c>
+      <c r="D121" t="s">
+        <v>176</v>
+      </c>
+      <c r="E121" t="s">
+        <v>176</v>
+      </c>
+      <c r="F121" t="s">
+        <v>64</v>
+      </c>
+      <c r="G121" t="s">
+        <v>149</v>
+      </c>
+      <c r="H121" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8">
+      <c r="A122" t="s">
+        <v>65</v>
+      </c>
+      <c r="B122" t="s">
+        <v>70</v>
+      </c>
+      <c r="C122" t="s">
+        <v>177</v>
+      </c>
+      <c r="D122" t="s">
+        <v>178</v>
+      </c>
+      <c r="E122" t="s">
+        <v>179</v>
+      </c>
+      <c r="F122" t="s">
+        <v>70</v>
+      </c>
+      <c r="G122" t="s">
+        <v>149</v>
+      </c>
+      <c r="H122" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8">
+      <c r="A123" t="s">
+        <v>71</v>
+      </c>
+      <c r="B123" t="s">
+        <v>72</v>
+      </c>
+      <c r="C123" t="s">
+        <v>73</v>
+      </c>
+      <c r="D123" t="s">
+        <v>74</v>
+      </c>
+      <c r="E123" t="s">
+        <v>75</v>
+      </c>
+      <c r="F123" t="s">
+        <v>76</v>
+      </c>
+      <c r="G123" t="s">
+        <v>149</v>
+      </c>
+      <c r="H123" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8">
+      <c r="A124" t="s">
+        <v>77</v>
+      </c>
+      <c r="B124" t="s">
+        <v>78</v>
+      </c>
+      <c r="C124" t="s">
+        <v>1</v>
+      </c>
+      <c r="D124" t="s">
+        <v>79</v>
+      </c>
+      <c r="E124" t="s">
+        <v>1</v>
+      </c>
+      <c r="F124" t="s">
+        <v>80</v>
+      </c>
+      <c r="G124" t="s">
+        <v>149</v>
+      </c>
+      <c r="H124" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8">
+      <c r="A125" t="s">
+        <v>81</v>
+      </c>
+      <c r="B125" t="s">
+        <v>82</v>
+      </c>
+      <c r="C125" t="s">
+        <v>83</v>
+      </c>
+      <c r="D125" t="s">
+        <v>84</v>
+      </c>
+      <c r="E125" t="s">
+        <v>85</v>
+      </c>
+      <c r="F125" t="s">
+        <v>51</v>
+      </c>
+      <c r="G125" t="s">
+        <v>149</v>
+      </c>
+      <c r="H125" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8">
+      <c r="A126" t="s">
+        <v>86</v>
+      </c>
+      <c r="B126" t="s">
+        <v>180</v>
+      </c>
+      <c r="C126" t="s">
+        <v>181</v>
+      </c>
+      <c r="D126" t="s">
+        <v>182</v>
+      </c>
+      <c r="E126" t="s">
+        <v>183</v>
+      </c>
+      <c r="F126" t="s">
+        <v>91</v>
+      </c>
+      <c r="G126" t="s">
+        <v>149</v>
+      </c>
+      <c r="H126" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8">
+      <c r="A127" t="s">
+        <v>92</v>
+      </c>
+      <c r="B127" t="s">
+        <v>184</v>
+      </c>
+      <c r="C127" t="s">
+        <v>185</v>
+      </c>
+      <c r="D127" t="s">
+        <v>186</v>
+      </c>
+      <c r="E127" t="s">
+        <v>187</v>
+      </c>
+      <c r="F127" t="s">
+        <v>97</v>
+      </c>
+      <c r="G127" t="s">
+        <v>149</v>
+      </c>
+      <c r="H127" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8">
+      <c r="A128" t="s">
+        <v>98</v>
+      </c>
+      <c r="B128" t="s">
+        <v>188</v>
+      </c>
+      <c r="C128" t="s">
+        <v>189</v>
+      </c>
+      <c r="D128" t="s">
+        <v>190</v>
+      </c>
+      <c r="E128" t="s">
+        <v>191</v>
+      </c>
+      <c r="F128" t="s">
+        <v>103</v>
+      </c>
+      <c r="G128" t="s">
+        <v>149</v>
+      </c>
+      <c r="H128" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8">
+      <c r="A129" t="s">
+        <v>104</v>
+      </c>
+      <c r="B129" t="s">
+        <v>1</v>
+      </c>
+      <c r="C129" t="s">
+        <v>105</v>
+      </c>
+      <c r="D129" t="s">
+        <v>1</v>
+      </c>
+      <c r="E129" t="s">
+        <v>106</v>
+      </c>
+      <c r="F129" t="s">
+        <v>107</v>
+      </c>
+      <c r="G129" t="s">
+        <v>149</v>
+      </c>
+      <c r="H129" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8">
+      <c r="A130" t="s">
+        <v>108</v>
+      </c>
+      <c r="B130" t="s">
+        <v>192</v>
+      </c>
+      <c r="C130" t="s">
+        <v>193</v>
+      </c>
+      <c r="D130" t="s">
+        <v>194</v>
+      </c>
+      <c r="E130" t="s">
+        <v>195</v>
+      </c>
+      <c r="F130" t="s">
+        <v>113</v>
+      </c>
+      <c r="G130" t="s">
+        <v>149</v>
+      </c>
+      <c r="H130" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8">
+      <c r="A131" t="s">
+        <v>114</v>
+      </c>
+      <c r="B131" t="s">
+        <v>196</v>
+      </c>
+      <c r="C131" t="s">
+        <v>197</v>
+      </c>
+      <c r="D131" t="s">
+        <v>198</v>
+      </c>
+      <c r="E131" t="s">
+        <v>199</v>
+      </c>
+      <c r="F131" t="s">
+        <v>119</v>
+      </c>
+      <c r="G131" t="s">
+        <v>149</v>
+      </c>
+      <c r="H131" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8">
+      <c r="A132" t="s">
+        <v>120</v>
+      </c>
+      <c r="B132" t="s">
+        <v>200</v>
+      </c>
+      <c r="C132" t="s">
+        <v>201</v>
+      </c>
+      <c r="D132" t="s">
+        <v>202</v>
+      </c>
+      <c r="E132" t="s">
+        <v>203</v>
+      </c>
+      <c r="F132" t="s">
+        <v>125</v>
+      </c>
+      <c r="G132" t="s">
+        <v>149</v>
+      </c>
+      <c r="H132" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8">
+      <c r="A133" t="s">
+        <v>126</v>
+      </c>
+      <c r="B133" t="s">
+        <v>204</v>
+      </c>
+      <c r="C133" t="s">
+        <v>205</v>
+      </c>
+      <c r="D133" t="s">
+        <v>206</v>
+      </c>
+      <c r="E133" t="s">
+        <v>207</v>
+      </c>
+      <c r="F133" t="s">
+        <v>131</v>
+      </c>
+      <c r="G133" t="s">
+        <v>149</v>
+      </c>
+      <c r="H133" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8">
+      <c r="A134" t="s">
+        <v>132</v>
+      </c>
+      <c r="B134" t="s">
+        <v>1</v>
+      </c>
+      <c r="C134" t="s">
+        <v>133</v>
+      </c>
+      <c r="D134" t="s">
+        <v>1</v>
+      </c>
+      <c r="E134" t="s">
+        <v>134</v>
+      </c>
+      <c r="F134" t="s">
+        <v>135</v>
+      </c>
+      <c r="G134" t="s">
+        <v>149</v>
+      </c>
+      <c r="H134" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8">
+      <c r="A135" t="s">
+        <v>136</v>
+      </c>
+      <c r="B135" t="s">
+        <v>137</v>
+      </c>
+      <c r="C135" t="s">
+        <v>138</v>
+      </c>
+      <c r="D135" t="s">
+        <v>139</v>
+      </c>
+      <c r="E135" t="s">
+        <v>139</v>
+      </c>
+      <c r="F135" t="s">
+        <v>140</v>
+      </c>
+      <c r="G135" t="s">
+        <v>149</v>
+      </c>
+      <c r="H135" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8">
+      <c r="A136" t="s">
+        <v>141</v>
+      </c>
+      <c r="B136" t="s">
+        <v>208</v>
+      </c>
+      <c r="C136" t="s">
+        <v>209</v>
+      </c>
+      <c r="D136" t="s">
+        <v>210</v>
+      </c>
+      <c r="E136" t="s">
+        <v>211</v>
+      </c>
+      <c r="F136" t="s">
+        <v>146</v>
+      </c>
+      <c r="G136" t="s">
+        <v>149</v>
+      </c>
+      <c r="H136" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8">
+      <c r="A137" t="s">
+        <v>0</v>
+      </c>
+      <c r="B137" t="s">
+        <v>1</v>
+      </c>
+      <c r="C137" t="s">
+        <v>147</v>
+      </c>
+      <c r="D137" t="s">
+        <v>1</v>
+      </c>
+      <c r="E137" t="s">
+        <v>148</v>
+      </c>
+      <c r="F137" t="s">
+        <v>4</v>
+      </c>
+      <c r="G137" t="s">
+        <v>149</v>
+      </c>
+      <c r="H137" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8">
+      <c r="A138" t="s">
+        <v>7</v>
+      </c>
+      <c r="B138" t="s">
+        <v>151</v>
+      </c>
+      <c r="C138" t="s">
+        <v>152</v>
+      </c>
+      <c r="D138" t="s">
+        <v>153</v>
+      </c>
+      <c r="E138" t="s">
+        <v>154</v>
+      </c>
+      <c r="F138" t="s">
+        <v>12</v>
+      </c>
+      <c r="G138" t="s">
+        <v>149</v>
+      </c>
+      <c r="H138" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8">
+      <c r="A139" t="s">
+        <v>13</v>
+      </c>
+      <c r="B139" t="s">
+        <v>1</v>
+      </c>
+      <c r="C139" t="s">
+        <v>14</v>
+      </c>
+      <c r="D139" t="s">
+        <v>1</v>
+      </c>
+      <c r="E139" t="s">
+        <v>15</v>
+      </c>
+      <c r="F139" t="s">
+        <v>16</v>
+      </c>
+      <c r="G139" t="s">
+        <v>149</v>
+      </c>
+      <c r="H139" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8">
+      <c r="A140" t="s">
+        <v>17</v>
+      </c>
+      <c r="B140" t="s">
+        <v>18</v>
+      </c>
+      <c r="C140" t="s">
+        <v>19</v>
+      </c>
+      <c r="D140" t="s">
+        <v>20</v>
+      </c>
+      <c r="E140" t="s">
+        <v>21</v>
+      </c>
+      <c r="F140" t="s">
+        <v>22</v>
+      </c>
+      <c r="G140" t="s">
+        <v>149</v>
+      </c>
+      <c r="H140" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8">
+      <c r="A141" t="s">
+        <v>23</v>
+      </c>
+      <c r="B141" t="s">
+        <v>155</v>
+      </c>
+      <c r="C141" t="s">
+        <v>156</v>
+      </c>
+      <c r="D141" t="s">
+        <v>157</v>
+      </c>
+      <c r="E141" t="s">
+        <v>158</v>
+      </c>
+      <c r="F141" t="s">
+        <v>28</v>
+      </c>
+      <c r="G141" t="s">
+        <v>149</v>
+      </c>
+      <c r="H141" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8">
+      <c r="A142" t="s">
+        <v>29</v>
+      </c>
+      <c r="B142" t="s">
+        <v>159</v>
+      </c>
+      <c r="C142" t="s">
+        <v>160</v>
+      </c>
+      <c r="D142" t="s">
+        <v>161</v>
+      </c>
+      <c r="E142" t="s">
+        <v>162</v>
+      </c>
+      <c r="F142" t="s">
+        <v>34</v>
+      </c>
+      <c r="G142" t="s">
+        <v>149</v>
+      </c>
+      <c r="H142" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8">
+      <c r="A143" t="s">
+        <v>35</v>
+      </c>
+      <c r="B143" t="s">
+        <v>163</v>
+      </c>
+      <c r="C143" t="s">
+        <v>164</v>
+      </c>
+      <c r="D143" t="s">
+        <v>165</v>
+      </c>
+      <c r="E143" t="s">
+        <v>166</v>
+      </c>
+      <c r="F143" t="s">
+        <v>40</v>
+      </c>
+      <c r="G143" t="s">
+        <v>149</v>
+      </c>
+      <c r="H143" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8">
+      <c r="A144" t="s">
+        <v>41</v>
+      </c>
+      <c r="B144" t="s">
+        <v>167</v>
+      </c>
+      <c r="C144" t="s">
+        <v>168</v>
+      </c>
+      <c r="D144" t="s">
+        <v>169</v>
+      </c>
+      <c r="E144" t="s">
+        <v>170</v>
+      </c>
+      <c r="F144" t="s">
+        <v>46</v>
+      </c>
+      <c r="G144" t="s">
+        <v>149</v>
+      </c>
+      <c r="H144" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8">
+      <c r="A145" t="s">
+        <v>47</v>
+      </c>
+      <c r="B145" t="s">
+        <v>171</v>
+      </c>
+      <c r="C145" t="s">
+        <v>172</v>
+      </c>
+      <c r="D145" t="s">
+        <v>173</v>
+      </c>
+      <c r="E145" t="s">
+        <v>173</v>
+      </c>
+      <c r="F145" t="s">
+        <v>51</v>
+      </c>
+      <c r="G145" t="s">
+        <v>149</v>
+      </c>
+      <c r="H145" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8">
+      <c r="A146" t="s">
+        <v>52</v>
+      </c>
+      <c r="B146" t="s">
+        <v>1</v>
+      </c>
+      <c r="C146" t="s">
+        <v>53</v>
+      </c>
+      <c r="D146" t="s">
+        <v>1</v>
+      </c>
+      <c r="E146" t="s">
+        <v>54</v>
+      </c>
+      <c r="F146" t="s">
+        <v>55</v>
+      </c>
+      <c r="G146" t="s">
+        <v>149</v>
+      </c>
+      <c r="H146" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8">
+      <c r="A147" t="s">
+        <v>56</v>
+      </c>
+      <c r="B147" t="s">
+        <v>1</v>
+      </c>
+      <c r="C147" t="s">
+        <v>57</v>
+      </c>
+      <c r="D147" t="s">
+        <v>1</v>
+      </c>
+      <c r="E147" t="s">
+        <v>58</v>
+      </c>
+      <c r="F147" t="s">
+        <v>59</v>
+      </c>
+      <c r="G147" t="s">
+        <v>149</v>
+      </c>
+      <c r="H147" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8">
+      <c r="A148" t="s">
+        <v>60</v>
+      </c>
+      <c r="B148" t="s">
+        <v>174</v>
+      </c>
+      <c r="C148" t="s">
+        <v>175</v>
+      </c>
+      <c r="D148" t="s">
+        <v>176</v>
+      </c>
+      <c r="E148" t="s">
+        <v>176</v>
+      </c>
+      <c r="F148" t="s">
+        <v>64</v>
+      </c>
+      <c r="G148" t="s">
+        <v>149</v>
+      </c>
+      <c r="H148" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8">
+      <c r="A149" t="s">
+        <v>65</v>
+      </c>
+      <c r="B149" t="s">
+        <v>70</v>
+      </c>
+      <c r="C149" t="s">
+        <v>177</v>
+      </c>
+      <c r="D149" t="s">
+        <v>178</v>
+      </c>
+      <c r="E149" t="s">
+        <v>179</v>
+      </c>
+      <c r="F149" t="s">
+        <v>70</v>
+      </c>
+      <c r="G149" t="s">
+        <v>149</v>
+      </c>
+      <c r="H149" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8">
+      <c r="A150" t="s">
+        <v>71</v>
+      </c>
+      <c r="B150" t="s">
+        <v>72</v>
+      </c>
+      <c r="C150" t="s">
+        <v>73</v>
+      </c>
+      <c r="D150" t="s">
+        <v>74</v>
+      </c>
+      <c r="E150" t="s">
+        <v>75</v>
+      </c>
+      <c r="F150" t="s">
+        <v>76</v>
+      </c>
+      <c r="G150" t="s">
+        <v>149</v>
+      </c>
+      <c r="H150" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8">
+      <c r="A151" t="s">
+        <v>77</v>
+      </c>
+      <c r="B151" t="s">
+        <v>78</v>
+      </c>
+      <c r="C151" t="s">
+        <v>1</v>
+      </c>
+      <c r="D151" t="s">
+        <v>79</v>
+      </c>
+      <c r="E151" t="s">
+        <v>1</v>
+      </c>
+      <c r="F151" t="s">
+        <v>80</v>
+      </c>
+      <c r="G151" t="s">
+        <v>149</v>
+      </c>
+      <c r="H151" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8">
+      <c r="A152" t="s">
+        <v>81</v>
+      </c>
+      <c r="B152" t="s">
+        <v>82</v>
+      </c>
+      <c r="C152" t="s">
+        <v>83</v>
+      </c>
+      <c r="D152" t="s">
+        <v>84</v>
+      </c>
+      <c r="E152" t="s">
+        <v>85</v>
+      </c>
+      <c r="F152" t="s">
+        <v>51</v>
+      </c>
+      <c r="G152" t="s">
+        <v>149</v>
+      </c>
+      <c r="H152" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8">
+      <c r="A153" t="s">
+        <v>86</v>
+      </c>
+      <c r="B153" t="s">
+        <v>180</v>
+      </c>
+      <c r="C153" t="s">
+        <v>181</v>
+      </c>
+      <c r="D153" t="s">
+        <v>182</v>
+      </c>
+      <c r="E153" t="s">
+        <v>183</v>
+      </c>
+      <c r="F153" t="s">
+        <v>91</v>
+      </c>
+      <c r="G153" t="s">
+        <v>149</v>
+      </c>
+      <c r="H153" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8">
+      <c r="A154" t="s">
+        <v>92</v>
+      </c>
+      <c r="B154" t="s">
+        <v>184</v>
+      </c>
+      <c r="C154" t="s">
+        <v>185</v>
+      </c>
+      <c r="D154" t="s">
+        <v>186</v>
+      </c>
+      <c r="E154" t="s">
+        <v>187</v>
+      </c>
+      <c r="F154" t="s">
+        <v>97</v>
+      </c>
+      <c r="G154" t="s">
+        <v>149</v>
+      </c>
+      <c r="H154" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8">
+      <c r="A155" t="s">
+        <v>98</v>
+      </c>
+      <c r="B155" t="s">
+        <v>188</v>
+      </c>
+      <c r="C155" t="s">
+        <v>189</v>
+      </c>
+      <c r="D155" t="s">
+        <v>190</v>
+      </c>
+      <c r="E155" t="s">
+        <v>191</v>
+      </c>
+      <c r="F155" t="s">
+        <v>103</v>
+      </c>
+      <c r="G155" t="s">
+        <v>149</v>
+      </c>
+      <c r="H155" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8">
+      <c r="A156" t="s">
+        <v>104</v>
+      </c>
+      <c r="B156" t="s">
+        <v>1</v>
+      </c>
+      <c r="C156" t="s">
+        <v>105</v>
+      </c>
+      <c r="D156" t="s">
+        <v>1</v>
+      </c>
+      <c r="E156" t="s">
+        <v>106</v>
+      </c>
+      <c r="F156" t="s">
+        <v>107</v>
+      </c>
+      <c r="G156" t="s">
+        <v>149</v>
+      </c>
+      <c r="H156" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8">
+      <c r="A157" t="s">
+        <v>108</v>
+      </c>
+      <c r="B157" t="s">
+        <v>192</v>
+      </c>
+      <c r="C157" t="s">
+        <v>193</v>
+      </c>
+      <c r="D157" t="s">
+        <v>194</v>
+      </c>
+      <c r="E157" t="s">
+        <v>195</v>
+      </c>
+      <c r="F157" t="s">
+        <v>113</v>
+      </c>
+      <c r="G157" t="s">
+        <v>149</v>
+      </c>
+      <c r="H157" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8">
+      <c r="A158" t="s">
+        <v>114</v>
+      </c>
+      <c r="B158" t="s">
+        <v>196</v>
+      </c>
+      <c r="C158" t="s">
+        <v>197</v>
+      </c>
+      <c r="D158" t="s">
+        <v>198</v>
+      </c>
+      <c r="E158" t="s">
+        <v>199</v>
+      </c>
+      <c r="F158" t="s">
+        <v>119</v>
+      </c>
+      <c r="G158" t="s">
+        <v>149</v>
+      </c>
+      <c r="H158" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8">
+      <c r="A159" t="s">
+        <v>120</v>
+      </c>
+      <c r="B159" t="s">
+        <v>200</v>
+      </c>
+      <c r="C159" t="s">
+        <v>201</v>
+      </c>
+      <c r="D159" t="s">
+        <v>202</v>
+      </c>
+      <c r="E159" t="s">
+        <v>203</v>
+      </c>
+      <c r="F159" t="s">
+        <v>125</v>
+      </c>
+      <c r="G159" t="s">
+        <v>149</v>
+      </c>
+      <c r="H159" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8">
+      <c r="A160" t="s">
+        <v>126</v>
+      </c>
+      <c r="B160" t="s">
+        <v>204</v>
+      </c>
+      <c r="C160" t="s">
+        <v>205</v>
+      </c>
+      <c r="D160" t="s">
+        <v>206</v>
+      </c>
+      <c r="E160" t="s">
+        <v>207</v>
+      </c>
+      <c r="F160" t="s">
+        <v>131</v>
+      </c>
+      <c r="G160" t="s">
+        <v>149</v>
+      </c>
+      <c r="H160" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8">
+      <c r="A161" t="s">
+        <v>132</v>
+      </c>
+      <c r="B161" t="s">
+        <v>1</v>
+      </c>
+      <c r="C161" t="s">
+        <v>133</v>
+      </c>
+      <c r="D161" t="s">
+        <v>1</v>
+      </c>
+      <c r="E161" t="s">
+        <v>134</v>
+      </c>
+      <c r="F161" t="s">
+        <v>135</v>
+      </c>
+      <c r="G161" t="s">
+        <v>149</v>
+      </c>
+      <c r="H161" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8">
+      <c r="A162" t="s">
+        <v>136</v>
+      </c>
+      <c r="B162" t="s">
+        <v>137</v>
+      </c>
+      <c r="C162" t="s">
+        <v>138</v>
+      </c>
+      <c r="D162" t="s">
+        <v>139</v>
+      </c>
+      <c r="E162" t="s">
+        <v>139</v>
+      </c>
+      <c r="F162" t="s">
+        <v>140</v>
+      </c>
+      <c r="G162" t="s">
+        <v>149</v>
+      </c>
+      <c r="H162" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8">
+      <c r="A163" t="s">
+        <v>141</v>
+      </c>
+      <c r="B163" t="s">
+        <v>208</v>
+      </c>
+      <c r="C163" t="s">
+        <v>209</v>
+      </c>
+      <c r="D163" t="s">
+        <v>210</v>
+      </c>
+      <c r="E163" t="s">
+        <v>211</v>
+      </c>
+      <c r="F163" t="s">
+        <v>146</v>
+      </c>
+      <c r="G163" t="s">
+        <v>149</v>
+      </c>
+      <c r="H163" t="s">
+        <v>150</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>